<commit_message>
modification of gene list (removal of those unavailable)
</commit_message>
<xml_diff>
--- a/gene_search/data/Bioinformatical analysis.xlsx
+++ b/gene_search/data/Bioinformatical analysis.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="983" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="983" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -765,7 +765,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -790,30 +790,6 @@
         <bgColor rgb="FFFF6600"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF009933"/>
-        <bgColor rgb="FF009900"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF990000"/>
-        <bgColor rgb="FF800000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF009900"/>
-        <bgColor rgb="FF009933"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border diagonalUp="false" diagonalDown="false">
@@ -852,7 +828,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="23">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -905,7 +881,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="9" fillId="4" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -937,19 +917,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -973,12 +941,12 @@
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF990000"/>
-      <rgbColor rgb="FF009900"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF006100"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF009933"/>
+      <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC0C0C0"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
@@ -1015,7 +983,7 @@
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF006100"/>
+      <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FF993300"/>
       <rgbColor rgb="FF993366"/>
@@ -1033,16 +1001,16 @@
   </sheetPr>
   <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29:C30"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F28" activeCellId="0" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="36.8520408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="33.8826530612245"/>
-    <col collapsed="false" hidden="false" max="9" min="3" style="1" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="36.4489795918367"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="33.4795918367347"/>
+    <col collapsed="false" hidden="false" max="9" min="3" style="1" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1594,7 +1562,7 @@
       <c r="B29" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="C29" s="11" t="s">
+      <c r="C29" s="13" t="s">
         <v>101</v>
       </c>
       <c r="D29" s="0" t="s">
@@ -1608,7 +1576,7 @@
       <c r="B30" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="C30" s="13" t="s">
+      <c r="C30" s="14" t="s">
         <v>105</v>
       </c>
       <c r="D30" s="0" t="s">
@@ -1622,7 +1590,7 @@
       <c r="D31" s="0"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="14" t="s">
+      <c r="A32" s="15" t="s">
         <v>106</v>
       </c>
       <c r="B32" s="4" t="s">
@@ -1706,7 +1674,7 @@
       <c r="D39" s="0"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="15" t="s">
+      <c r="A40" s="16" t="s">
         <v>115</v>
       </c>
       <c r="B40" s="0"/>
@@ -1720,7 +1688,7 @@
       <c r="B41" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="C41" s="16" t="s">
+      <c r="C41" s="17" t="s">
         <v>117</v>
       </c>
       <c r="D41" s="0"/>
@@ -1732,7 +1700,7 @@
       <c r="B42" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="C42" s="16" t="s">
+      <c r="C42" s="17" t="s">
         <v>119</v>
       </c>
       <c r="D42" s="0"/>
@@ -1758,7 +1726,7 @@
       <c r="B45" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="C45" s="17" t="s">
+      <c r="C45" s="18" t="s">
         <v>123</v>
       </c>
       <c r="D45" s="0"/>
@@ -1770,7 +1738,7 @@
       <c r="B46" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="C46" s="16" t="s">
+      <c r="C46" s="17" t="s">
         <v>125</v>
       </c>
       <c r="D46" s="0"/>
@@ -1782,7 +1750,7 @@
       <c r="B47" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="C47" s="16" t="s">
+      <c r="C47" s="17" t="s">
         <v>127</v>
       </c>
       <c r="D47" s="0"/>
@@ -1794,13 +1762,13 @@
       <c r="D48" s="0"/>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="18" t="s">
+      <c r="A49" s="19" t="s">
         <v>128</v>
       </c>
       <c r="B49" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="C49" s="16" t="s">
+      <c r="C49" s="17" t="s">
         <v>129</v>
       </c>
       <c r="D49" s="0"/>
@@ -1812,13 +1780,13 @@
       <c r="D50" s="0"/>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="18" t="s">
+      <c r="A51" s="19" t="s">
         <v>130</v>
       </c>
-      <c r="B51" s="19" t="s">
+      <c r="B51" s="20" t="s">
         <v>131</v>
       </c>
-      <c r="C51" s="19" t="s">
+      <c r="C51" s="20" t="s">
         <v>132</v>
       </c>
       <c r="D51" s="1" t="s">
@@ -1826,13 +1794,13 @@
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="20" t="s">
+      <c r="A52" s="21" t="s">
         <v>134</v>
       </c>
-      <c r="B52" s="20" t="s">
+      <c r="B52" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="C52" s="16" t="s">
+      <c r="C52" s="17" t="s">
         <v>135</v>
       </c>
     </row>
@@ -1842,13 +1810,13 @@
       <c r="C53" s="0"/>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="18" t="s">
+      <c r="A54" s="19" t="s">
         <v>136</v>
       </c>
-      <c r="B54" s="20" t="s">
+      <c r="B54" s="21" t="s">
         <v>137</v>
       </c>
-      <c r="C54" s="19" t="s">
+      <c r="C54" s="20" t="s">
         <v>138</v>
       </c>
     </row>
@@ -1870,43 +1838,43 @@
   </sheetPr>
   <dimension ref="A1:A66"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="1" sqref="C29:C30 A7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.9030612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.8010204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="22" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="22" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="22" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="22" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="22" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="22" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1926,32 +1894,32 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="23" t="s">
+      <c r="A10" s="22" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="22" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="22" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="23" t="s">
+      <c r="A13" s="22" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="23" t="s">
+      <c r="A14" s="22" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="23" t="s">
+      <c r="A15" s="22" t="s">
         <v>30</v>
       </c>
     </row>
@@ -2001,47 +1969,47 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="23" t="s">
+      <c r="A25" s="22" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="23" t="s">
+      <c r="A26" s="22" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="23" t="s">
+      <c r="A27" s="22" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="23" t="s">
+      <c r="A28" s="22" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="23" t="s">
+      <c r="A29" s="22" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="24" t="s">
+      <c r="A30" s="22" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="24" t="s">
+      <c r="A31" s="22" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="24" t="s">
+      <c r="A32" s="22" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="24" t="s">
+      <c r="A33" s="22" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2061,142 +2029,142 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="23" t="s">
+      <c r="A37" s="22" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="23" t="s">
+      <c r="A38" s="22" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="23" t="s">
+      <c r="A39" s="22" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="23" t="s">
+      <c r="A40" s="22" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="23" t="s">
+      <c r="A41" s="22" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="23" t="s">
+      <c r="A42" s="22" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="23" t="s">
+      <c r="A43" s="22" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="23" t="s">
+      <c r="A44" s="22" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="23" t="s">
+      <c r="A45" s="22" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="23" t="s">
+      <c r="A46" s="22" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="23" t="s">
+      <c r="A47" s="22" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="23" t="s">
+      <c r="A48" s="22" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="23" t="s">
+      <c r="A49" s="22" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="24" t="s">
+      <c r="A50" s="22" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="23" t="s">
+      <c r="A51" s="22" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="23" t="s">
+      <c r="A52" s="22" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="22" t="s">
+      <c r="A53" s="14" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="22" t="s">
+      <c r="A54" s="14" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="23" t="s">
+      <c r="A55" s="22" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="23" t="s">
+      <c r="A56" s="22" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="23" t="s">
+      <c r="A57" s="22" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="23" t="s">
+      <c r="A58" s="22" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="23" t="s">
+      <c r="A59" s="22" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="23" t="s">
+      <c r="A60" s="22" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="23" t="s">
+      <c r="A61" s="22" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="23" t="s">
+      <c r="A62" s="22" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="23" t="s">
+      <c r="A63" s="22" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="23" t="s">
+      <c r="A64" s="22" t="s">
         <v>129</v>
       </c>
     </row>
@@ -2206,7 +2174,7 @@
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="22" t="s">
+      <c r="A66" s="14" t="s">
         <v>138</v>
       </c>
     </row>

</xml_diff>